<commit_message>
Stable commit: Added exclude user list, irrelevant filter, picture display feature.
Also fixed some bugs of display of reply.
</commit_message>
<xml_diff>
--- a/comments.xlsx
+++ b/comments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4dad9766b93e19e1/桌面/CommentFilterPrototype/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTMLandPython\CommentFilterPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_304384039EA2033220C3872D58297F65F1E2351D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F96F2052-7313-4E55-9A7A-DB8A21B4A01D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195643A0-5D75-40E0-AFA1-3BC3068BBA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mainComments" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -120,13 +120,47 @@
   </si>
   <si>
     <t>2025-05-27 10:14</t>
+  </si>
+  <si>
+    <t>irrelevantTag</t>
+  </si>
+  <si>
+    <t>image</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿扁</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>三小</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025-05-27 10:16</t>
+  </si>
+  <si>
+    <t>蛤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pic3.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pic2.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pic4.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +181,13 @@
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,12 +225,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -494,18 +538,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.5" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.5" defaultRowHeight="28.5" customHeight="1"/>
   <cols>
     <col min="1" max="16384" width="17.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,8 +568,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.5" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -545,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28.5" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -564,8 +614,11 @@
       <c r="F3" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.5" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -584,8 +637,11 @@
       <c r="F4" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.5" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -605,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -623,6 +679,29 @@
       </c>
       <c r="F6" s="2">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" customHeight="1">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -633,18 +712,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.5" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="17.5" defaultRowHeight="28.5" customHeight="1"/>
   <cols>
     <col min="1" max="16384" width="17.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -663,8 +742,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.5" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -683,8 +768,11 @@
       <c r="F2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.5" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -703,8 +791,11 @@
       <c r="F3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.5" customHeight="1">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -724,7 +815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.5" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -742,6 +833,32 @@
       </c>
       <c r="F5" s="2">
         <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" customHeight="1">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stable commit: Added AI keyword filter feature.
Fixed more bugs, and make some UI more consistent.
Reorganized some function, button bind and style in css.
</commit_message>
<xml_diff>
--- a/comments.xlsx
+++ b/comments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTMLandPython\CommentFilterPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195643A0-5D75-40E0-AFA1-3BC3068BBA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77276EF-FA56-466A-A304-EC1D62A2734D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mainComments" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -153,6 +153,10 @@
   </si>
   <si>
     <t>pic4.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pic1.jpg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -540,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5" defaultRowHeight="28.5" customHeight="1"/>
@@ -594,6 +598,9 @@
       <c r="F2" s="2">
         <v>2</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="28.5" customHeight="1">
       <c r="A3" s="2">
@@ -714,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5" defaultRowHeight="28.5" customHeight="1"/>

</xml_diff>

<commit_message>
Added some actual picture url to forms.
</commit_message>
<xml_diff>
--- a/comments.xlsx
+++ b/comments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTMLandPython\CommentFilterPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A804146-4A31-467B-A3B2-A8CEED67C372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0926C2-31AD-4240-89F5-A8B3A39AD51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="25780" windowHeight="13860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mainComments" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="260">
   <si>
     <t>id</t>
   </si>
@@ -194,9 +194,6 @@
     <t>雖然Switch 2首銷成績亮眼不過遊戲陣容還不夠強，我猶豫要不要買。</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=img14</t>
-  </si>
-  <si>
     <t>遊戲迷</t>
   </si>
   <si>
@@ -335,9 +332,6 @@
     <t>2025-06-10 13:16:05</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=img30</t>
-  </si>
-  <si>
     <t>🐱</t>
   </si>
   <si>
@@ -353,9 +347,6 @@
     <t>感覺Switch2定位跟以前不太一樣，未來走向值得關注。</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=img32</t>
-  </si>
-  <si>
     <t>2025-06-10 13:44:33</t>
   </si>
   <si>
@@ -425,9 +416,6 @@
     <t>房仲看過來，超低月付房屋出租！</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=img42</t>
-  </si>
-  <si>
     <t>2025-06-10 14:54:58</t>
   </si>
   <si>
@@ -488,9 +476,6 @@
     <t>這主機真厲害！作為任天堂粉，我已經等不及了！</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=reply2</t>
-  </si>
-  <si>
     <t>2025-06-10 08:48:28</t>
   </si>
   <si>
@@ -515,9 +500,6 @@
     <t>Switch2的性能看來不錯，希望實機驗收能符合預期。</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=reply6</t>
-  </si>
-  <si>
     <t>2025-06-10 08:53:26</t>
   </si>
   <si>
@@ -578,9 +560,6 @@
     <t>消息說是三倍PS4，感覺有點誇張，可能包括預購數？</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=reply16</t>
-  </si>
-  <si>
     <t>2025-06-10 09:22:55</t>
   </si>
   <si>
@@ -713,18 +692,12 @@
     <t>Switch2很適合多人遊戲，一家大小一起玩很有趣。</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=reply37</t>
-  </si>
-  <si>
     <t>2025-06-10 12:58:18</t>
   </si>
   <si>
     <t>PS粉們應該很難接受這麼明顯的差距吧？</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=reply38</t>
-  </si>
-  <si>
     <t>2025-06-10 13:03:04</t>
   </si>
   <si>
@@ -797,8 +770,37 @@
     <t>我的Switch1還在用，相信Switch2的兼容性很重要。</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150?text=img26</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcS_2aj-qIkkLtRUvvPWlWtqRknJ2fOkfBfvpg&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSN5uKeAfny8LofPHK1YzXNk7eQC43ZF2F1ig&amp;s</t>
+  </si>
+  <si>
+    <t>https://cdn.unwire.hk/wp-content/uploads/2025/04/bafkreihd4pjfb4kambw.jpg</t>
+  </si>
+  <si>
+    <t>https://static.mianbaoban-assets.eet-china.com/xinyu-images/MBXY-CR-204b8815e764ae64927a39adabb6faab.png</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTw4nylq17SbvzSxxfPyM2s0a0G6w0Z3hoQeA&amp;s</t>
+  </si>
+  <si>
+    <t>https://www.coolpc.tw/tw/wp-content//uploads/2024/07/coolpc-vivobook-s15-s5507-67-700x700.jpg</t>
+  </si>
+  <si>
+    <t>https://www.koc.com.tw/wp-content/uploads/2022/12/1672236456-6c05c8f322e08d62989cdd834ea50f01.png</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSKCAYjPueE9Ytrf8iW-XOljXifgLSC_0_HzQ&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTgU21V0DKn4GFZ66v1hd2yyH9SlaPypMgv-A&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTHNflITDyDuo2ahwf7Zi1VKOhlCR8gQon0OA&amp;s</t>
+  </si>
+  <si>
+    <t>https://i0.wp.com/myfone.blog/wp-content/uploads/2024/05/Nintendo-Switch-Header-1-840w-472h.jpg.jpg?resize=747%2C420&amp;ssl=1</t>
   </si>
 </sst>
 </file>
@@ -1183,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -1538,7 +1540,7 @@
         <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>251</v>
       </c>
       <c r="H15" t="s">
         <v>12</v>
@@ -1549,16 +1551,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
       </c>
       <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
         <v>59</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
       </c>
       <c r="F16">
         <v>16</v>
@@ -1572,16 +1574,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
         <v>61</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>62</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>63</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
       </c>
       <c r="F17">
         <v>20</v>
@@ -1595,16 +1597,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>66</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>67</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
       </c>
       <c r="F18">
         <v>4</v>
@@ -1618,16 +1620,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
         <v>32</v>
       </c>
       <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
         <v>70</v>
-      </c>
-      <c r="E19" t="s">
-        <v>71</v>
       </c>
       <c r="F19">
         <v>17</v>
@@ -1641,16 +1643,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
         <v>72</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>73</v>
-      </c>
-      <c r="E20" t="s">
-        <v>74</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1664,16 +1666,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
         <v>75</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>76</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>77</v>
-      </c>
-      <c r="E21" t="s">
-        <v>78</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1693,10 +1695,10 @@
         <v>43</v>
       </c>
       <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" t="s">
         <v>79</v>
-      </c>
-      <c r="E22" t="s">
-        <v>80</v>
       </c>
       <c r="F22">
         <v>3</v>
@@ -1710,16 +1712,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
         <v>81</v>
-      </c>
-      <c r="E23" t="s">
-        <v>82</v>
       </c>
       <c r="F23">
         <v>7</v>
@@ -1733,16 +1735,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>84</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>85</v>
-      </c>
-      <c r="E24" t="s">
-        <v>86</v>
       </c>
       <c r="F24">
         <v>18</v>
@@ -1756,16 +1758,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25">
         <v>15</v>
@@ -1779,16 +1781,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
       <c r="D26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" t="s">
         <v>90</v>
-      </c>
-      <c r="E26" t="s">
-        <v>91</v>
       </c>
       <c r="F26">
         <v>17</v>
@@ -1802,22 +1804,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
       </c>
       <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
         <v>92</v>
-      </c>
-      <c r="E27" t="s">
-        <v>93</v>
       </c>
       <c r="F27">
         <v>4</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="H27" t="s">
         <v>12</v>
@@ -1831,13 +1833,13 @@
         <v>46</v>
       </c>
       <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" t="s">
         <v>94</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>95</v>
-      </c>
-      <c r="E28" t="s">
-        <v>96</v>
       </c>
       <c r="F28">
         <v>17</v>
@@ -1851,16 +1853,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
         <v>98</v>
-      </c>
-      <c r="E29" t="s">
-        <v>99</v>
       </c>
       <c r="F29">
         <v>16</v>
@@ -1874,16 +1876,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
         <v>75</v>
       </c>
-      <c r="C30" t="s">
-        <v>76</v>
-      </c>
       <c r="D30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" t="s">
         <v>100</v>
-      </c>
-      <c r="E30" t="s">
-        <v>101</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1897,22 +1899,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
         <v>102</v>
       </c>
-      <c r="C31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" t="s">
-        <v>103</v>
-      </c>
       <c r="E31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F31">
         <v>9</v>
       </c>
       <c r="G31" t="s">
-        <v>104</v>
+        <v>250</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
@@ -1926,13 +1928,13 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" t="s">
         <v>105</v>
-      </c>
-      <c r="D32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" t="s">
-        <v>107</v>
       </c>
       <c r="F32">
         <v>14</v>
@@ -1946,22 +1948,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
         <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F33">
         <v>3</v>
-      </c>
-      <c r="G33" t="s">
-        <v>110</v>
       </c>
       <c r="H33" t="s">
         <v>12</v>
@@ -1975,13 +1974,13 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -2001,10 +2000,10 @@
         <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E35" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F35">
         <v>18</v>
@@ -2018,19 +2017,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
         <v>75</v>
       </c>
-      <c r="C36" t="s">
-        <v>76</v>
-      </c>
       <c r="D36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F36">
         <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>252</v>
       </c>
       <c r="H36" t="s">
         <v>12</v>
@@ -2041,16 +2043,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2064,16 +2066,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F38">
         <v>7</v>
@@ -2087,16 +2089,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" t="s">
         <v>120</v>
       </c>
-      <c r="D39" t="s">
-        <v>123</v>
-      </c>
       <c r="E39" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F39">
         <v>10</v>
@@ -2110,16 +2112,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" t="s">
         <v>75</v>
       </c>
-      <c r="C40" t="s">
-        <v>76</v>
-      </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2133,16 +2135,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" t="s">
         <v>127</v>
-      </c>
-      <c r="C41" t="s">
-        <v>128</v>
-      </c>
-      <c r="D41" t="s">
-        <v>129</v>
-      </c>
-      <c r="E41" t="s">
-        <v>130</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2159,13 +2161,13 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2179,22 +2181,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E43" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>134</v>
+        <v>253</v>
       </c>
       <c r="H43" t="s">
         <v>12</v>
@@ -2205,16 +2207,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -2228,19 +2230,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D45" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E45" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F45">
         <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>254</v>
       </c>
       <c r="H45" t="s">
         <v>12</v>
@@ -2251,16 +2256,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D46" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E46" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2274,16 +2279,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" t="s">
         <v>28</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E47" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -2297,16 +2302,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D48" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E48" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -2320,16 +2325,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D49" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -2343,16 +2348,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" t="s">
         <v>75</v>
       </c>
-      <c r="C50" t="s">
-        <v>76</v>
-      </c>
       <c r="D50" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E50" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -2369,13 +2374,13 @@
         <v>27</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D51" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E51" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2386,9 +2391,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="G27" r:id="rId1" xr:uid="{2D4E2A21-9684-4452-974B-EDD00C192909}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2397,18 +2399,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="87.8984375" customWidth="1"/>
+    <col min="7" max="7" width="43.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -2437,13 +2440,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -2460,10 +2463,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -2483,22 +2486,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
         <v>65</v>
-      </c>
-      <c r="E4" t="s">
-        <v>66</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>155</v>
+        <v>259</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -2509,16 +2512,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2532,13 +2535,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -2555,13 +2558,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -2578,22 +2581,22 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>164</v>
+        <v>258</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
@@ -2604,13 +2607,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -2627,16 +2630,16 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F10">
         <v>6</v>
@@ -2650,16 +2653,16 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -2673,16 +2676,16 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -2696,13 +2699,13 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -2719,10 +2722,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
@@ -2742,16 +2745,16 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C15" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -2765,16 +2768,16 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D16" t="s">
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16">
         <v>7</v>
@@ -2788,10 +2791,10 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D17" t="s">
         <v>27</v>
@@ -2811,22 +2814,22 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C18" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18">
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>185</v>
+        <v>257</v>
       </c>
       <c r="H18" t="s">
         <v>12</v>
@@ -2837,10 +2840,10 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C19" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D19" t="s">
         <v>38</v>
@@ -2860,13 +2863,13 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C20" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
         <v>20</v>
@@ -2883,13 +2886,13 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C21" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
@@ -2906,10 +2909,10 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -2929,13 +2932,13 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C23" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E23" t="s">
         <v>28</v>
@@ -2952,10 +2955,10 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C24" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D24" t="s">
         <v>35</v>
@@ -2975,13 +2978,13 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C25" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
         <v>9</v>
@@ -2998,16 +3001,16 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C26" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D26" t="s">
         <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26">
         <v>5</v>
@@ -3021,16 +3024,16 @@
         <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C27" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -3044,16 +3047,16 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="F28">
         <v>12</v>
@@ -3067,16 +3070,16 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C29" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -3090,13 +3093,13 @@
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
@@ -3113,16 +3116,16 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C31" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F31">
         <v>7</v>
@@ -3136,16 +3139,16 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F32">
         <v>6</v>
@@ -3159,10 +3162,10 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C33" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D33" t="s">
         <v>49</v>
@@ -3182,16 +3185,16 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C34" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F34">
         <v>11</v>
@@ -3205,13 +3208,13 @@
         <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C35" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E35" t="s">
         <v>24</v>
@@ -3228,16 +3231,16 @@
         <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D36" t="s">
         <v>46</v>
       </c>
       <c r="E36" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F36">
         <v>7</v>
@@ -3251,13 +3254,13 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C37" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D37" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E37" t="s">
         <v>9</v>
@@ -3274,16 +3277,16 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C38" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D38" t="s">
         <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -3297,10 +3300,10 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C39" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -3312,7 +3315,7 @@
         <v>6</v>
       </c>
       <c r="G39" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="H39" t="s">
         <v>12</v>
@@ -3323,22 +3326,22 @@
         <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C40" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D40" t="s">
         <v>42</v>
       </c>
       <c r="E40" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="F40">
         <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -3349,10 +3352,10 @@
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C41" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D41" t="s">
         <v>38</v>
@@ -3372,10 +3375,10 @@
         <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C42" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
@@ -3395,10 +3398,10 @@
         <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C43" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D43" t="s">
         <v>46</v>
@@ -3418,10 +3421,10 @@
         <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C44" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="D44" t="s">
         <v>31</v>
@@ -3441,16 +3444,16 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C45" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="D45" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E45" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F45">
         <v>11</v>
@@ -3464,13 +3467,13 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C46" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="D46" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E46" t="s">
         <v>43</v>
@@ -3487,10 +3490,10 @@
         <v>34</v>
       </c>
       <c r="B47" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C47" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -3510,13 +3513,13 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C48" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E48" t="s">
         <v>24</v>
@@ -3533,13 +3536,13 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C49" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="D49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E49" t="s">
         <v>20</v>
@@ -3556,16 +3559,16 @@
         <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C50" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="D50" t="s">
         <v>54</v>
       </c>
       <c r="E50" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F50">
         <v>8</v>
@@ -3579,16 +3582,16 @@
         <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C51" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D51" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F51">
         <v>5</v>

</xml_diff>

<commit_message>
Milestone commit: Added questionnaire link and button to prototype. Basically finished.
</commit_message>
<xml_diff>
--- a/comments.xlsx
+++ b/comments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTMLandPython\CommentFilterPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0926C2-31AD-4240-89F5-A8B3A39AD51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0236AC17-608E-407B-8E7F-B6ABAA4D7B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mainComments" sheetId="1" r:id="rId1"/>
@@ -1185,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
@@ -2399,7 +2399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>